<commit_message>
used: pdf reader and finish-LP bot
</commit_message>
<xml_diff>
--- a/Open-LPs - deitado.xlsx
+++ b/Open-LPs - deitado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8551809-1CDF-4DBA-8998-5FEF07CD772D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCD82E4-E4CB-4C97-AF5D-37BEAFBEA88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>LP</t>
   </si>
@@ -28,217 +28,259 @@
     <t>Status</t>
   </si>
   <si>
-    <t>LP-040775</t>
-  </si>
-  <si>
-    <t>LP-041266</t>
-  </si>
-  <si>
-    <t>LP-043258</t>
-  </si>
-  <si>
-    <t>LP-045183</t>
-  </si>
-  <si>
-    <t>LP-045187</t>
-  </si>
-  <si>
-    <t>LP-045610</t>
-  </si>
-  <si>
-    <t>LP-046344</t>
-  </si>
-  <si>
-    <t>LP-046609</t>
-  </si>
-  <si>
-    <t>LP-046610</t>
-  </si>
-  <si>
-    <t>LP-046612</t>
-  </si>
-  <si>
-    <t>LP-046806</t>
-  </si>
-  <si>
-    <t>LP-047049</t>
-  </si>
-  <si>
-    <t>LP-047212</t>
-  </si>
-  <si>
-    <t>LP-047302</t>
-  </si>
-  <si>
-    <t>LP-047303</t>
-  </si>
-  <si>
-    <t>LP-047758</t>
-  </si>
-  <si>
-    <t>LP-047916</t>
-  </si>
-  <si>
-    <t>LP-048004</t>
-  </si>
-  <si>
-    <t>LP-048055</t>
-  </si>
-  <si>
-    <t>LP-048057</t>
-  </si>
-  <si>
-    <t>LP-048224</t>
-  </si>
-  <si>
-    <t>LP-048417</t>
-  </si>
-  <si>
-    <t>LP-048517</t>
-  </si>
-  <si>
-    <t>LP-048522</t>
-  </si>
-  <si>
-    <t>LP-048759</t>
-  </si>
-  <si>
-    <t>LP-048771</t>
-  </si>
-  <si>
-    <t>LP-048857</t>
-  </si>
-  <si>
-    <t>LP-040879</t>
-  </si>
-  <si>
-    <t>LP-048889</t>
-  </si>
-  <si>
-    <t>LP-043989</t>
-  </si>
-  <si>
-    <t>LP-046343</t>
-  </si>
-  <si>
-    <t>LP-046345</t>
-  </si>
-  <si>
-    <t>LP-046603</t>
-  </si>
-  <si>
-    <t>LP-046613</t>
-  </si>
-  <si>
-    <t>LP-046941</t>
-  </si>
-  <si>
-    <t>LP-047169</t>
-  </si>
-  <si>
-    <t>LP-047369</t>
-  </si>
-  <si>
-    <t>LP-047389</t>
-  </si>
-  <si>
-    <t>LP-047525</t>
-  </si>
-  <si>
-    <t>LP-047541</t>
-  </si>
-  <si>
-    <t>LP-047737</t>
-  </si>
-  <si>
-    <t>LP-047913</t>
-  </si>
-  <si>
-    <t>LP-048056</t>
-  </si>
-  <si>
-    <t>LP-048058</t>
-  </si>
-  <si>
-    <t>LP-048059</t>
-  </si>
-  <si>
-    <t>LP-048127</t>
-  </si>
-  <si>
-    <t>LP-048134</t>
-  </si>
-  <si>
-    <t>LP-048311</t>
-  </si>
-  <si>
-    <t>LP-048312</t>
-  </si>
-  <si>
-    <t>LP-048316</t>
-  </si>
-  <si>
-    <t>LP-048318</t>
-  </si>
-  <si>
-    <t>LP-048332</t>
-  </si>
-  <si>
-    <t>LP-048533</t>
-  </si>
-  <si>
-    <t>LP-048547</t>
-  </si>
-  <si>
-    <t>LP-048616</t>
-  </si>
-  <si>
-    <t>LP-048818</t>
-  </si>
-  <si>
-    <t>LP-048874</t>
-  </si>
-  <si>
-    <t>LP-047028</t>
-  </si>
-  <si>
-    <t>LP-047533</t>
-  </si>
-  <si>
-    <t>LP-047739</t>
-  </si>
-  <si>
-    <t>LP-047765</t>
-  </si>
-  <si>
-    <t>LP-048581</t>
-  </si>
-  <si>
-    <t>LP-048925</t>
-  </si>
-  <si>
-    <t>LP-046807</t>
-  </si>
-  <si>
-    <t>LP-046936</t>
-  </si>
-  <si>
-    <t>LP-047764</t>
-  </si>
-  <si>
-    <t>LP-048016</t>
-  </si>
-  <si>
-    <t>LP-048501</t>
-  </si>
-  <si>
-    <t>LP-047348</t>
-  </si>
-  <si>
-    <t>LP-047979</t>
-  </si>
-  <si>
-    <t>LP-048537</t>
+    <t>LP-039797</t>
+  </si>
+  <si>
+    <t>LP-043163</t>
+  </si>
+  <si>
+    <t>LP-043708</t>
+  </si>
+  <si>
+    <t>LP-044099</t>
+  </si>
+  <si>
+    <t>LP-044472</t>
+  </si>
+  <si>
+    <t>LP-044474</t>
+  </si>
+  <si>
+    <t>LP-046657</t>
+  </si>
+  <si>
+    <t>LP-047013</t>
+  </si>
+  <si>
+    <t>LP-047015</t>
+  </si>
+  <si>
+    <t>LP-047137</t>
+  </si>
+  <si>
+    <t>LP-047139</t>
+  </si>
+  <si>
+    <t>LP-047140</t>
+  </si>
+  <si>
+    <t>LP-047141</t>
+  </si>
+  <si>
+    <t>LP-047142</t>
+  </si>
+  <si>
+    <t>LP-047143</t>
+  </si>
+  <si>
+    <t>LP-047225</t>
+  </si>
+  <si>
+    <t>LP-047282</t>
+  </si>
+  <si>
+    <t>LP-047315</t>
+  </si>
+  <si>
+    <t>LP-047418</t>
+  </si>
+  <si>
+    <t>LP-047624</t>
+  </si>
+  <si>
+    <t>LP-047651</t>
+  </si>
+  <si>
+    <t>LP-047713</t>
+  </si>
+  <si>
+    <t>LP-047912</t>
+  </si>
+  <si>
+    <t>LP-043008</t>
+  </si>
+  <si>
+    <t>LP-048112</t>
+  </si>
+  <si>
+    <t>LP-048113</t>
+  </si>
+  <si>
+    <t>LP-048242</t>
+  </si>
+  <si>
+    <t>LP-048243</t>
+  </si>
+  <si>
+    <t>LP-048247</t>
+  </si>
+  <si>
+    <t>LP-048300</t>
+  </si>
+  <si>
+    <t>LP-048443</t>
+  </si>
+  <si>
+    <t>LP-048499</t>
+  </si>
+  <si>
+    <t>LP-048514</t>
+  </si>
+  <si>
+    <t>LP-048527</t>
+  </si>
+  <si>
+    <t>LP-048528</t>
+  </si>
+  <si>
+    <t>LP-048530</t>
+  </si>
+  <si>
+    <t>LP-048531</t>
+  </si>
+  <si>
+    <t>LP-048632</t>
+  </si>
+  <si>
+    <t>LP-048637</t>
+  </si>
+  <si>
+    <t>LP-048671</t>
+  </si>
+  <si>
+    <t>LP-048843</t>
+  </si>
+  <si>
+    <t>LP-048844</t>
+  </si>
+  <si>
+    <t>LP-048845</t>
+  </si>
+  <si>
+    <t>LP-048849</t>
+  </si>
+  <si>
+    <t>LP-049060</t>
+  </si>
+  <si>
+    <t>LP-049061</t>
+  </si>
+  <si>
+    <t>LP-046637</t>
+  </si>
+  <si>
+    <t>LP-047138</t>
+  </si>
+  <si>
+    <t>LP-047531</t>
+  </si>
+  <si>
+    <t>LP-047534</t>
+  </si>
+  <si>
+    <t>LP-047902</t>
+  </si>
+  <si>
+    <t>LP-047956</t>
+  </si>
+  <si>
+    <t>LP-047993</t>
+  </si>
+  <si>
+    <t>LP-048115</t>
+  </si>
+  <si>
+    <t>LP-048116</t>
+  </si>
+  <si>
+    <t>LP-048130</t>
+  </si>
+  <si>
+    <t>LP-048236</t>
+  </si>
+  <si>
+    <t>LP-048241</t>
+  </si>
+  <si>
+    <t>LP-048335</t>
+  </si>
+  <si>
+    <t>LP-048336</t>
+  </si>
+  <si>
+    <t>LP-048341</t>
+  </si>
+  <si>
+    <t>LP-048342</t>
+  </si>
+  <si>
+    <t>LP-048442</t>
+  </si>
+  <si>
+    <t>LP-048529</t>
+  </si>
+  <si>
+    <t>LP-048535</t>
+  </si>
+  <si>
+    <t>LP-048538</t>
+  </si>
+  <si>
+    <t>LP-048539</t>
+  </si>
+  <si>
+    <t>LP-048541</t>
+  </si>
+  <si>
+    <t>LP-048573</t>
+  </si>
+  <si>
+    <t>LP-048947</t>
+  </si>
+  <si>
+    <t>LP-048948</t>
+  </si>
+  <si>
+    <t>LP-048958</t>
+  </si>
+  <si>
+    <t>LP-049276</t>
+  </si>
+  <si>
+    <t>LP-043682</t>
+  </si>
+  <si>
+    <t>LP-048246</t>
+  </si>
+  <si>
+    <t>LP-048521</t>
+  </si>
+  <si>
+    <t>LP-048536</t>
+  </si>
+  <si>
+    <t>LP-048668</t>
+  </si>
+  <si>
+    <t>LP-047904</t>
+  </si>
+  <si>
+    <t>LP-048534</t>
+  </si>
+  <si>
+    <t>LP-048624</t>
+  </si>
+  <si>
+    <t>LP-047532</t>
+  </si>
+  <si>
+    <t>LP-047711</t>
+  </si>
+  <si>
+    <t>LP-048114</t>
+  </si>
+  <si>
+    <t>LP-048129</t>
   </si>
 </sst>
 </file>
@@ -601,7 +643,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -630,12 +672,12 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -655,7 +697,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -665,312 +707,382 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: pdf readers and finish bots updated
</commit_message>
<xml_diff>
--- a/Open-LPs - deitado.xlsx
+++ b/Open-LPs - deitado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCD82E4-E4CB-4C97-AF5D-37BEAFBEA88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6664EC-AAFB-4163-A7CA-AA7F28E85E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>LP</t>
   </si>
@@ -28,259 +28,214 @@
     <t>Status</t>
   </si>
   <si>
-    <t>LP-039797</t>
-  </si>
-  <si>
-    <t>LP-043163</t>
-  </si>
-  <si>
-    <t>LP-043708</t>
-  </si>
-  <si>
-    <t>LP-044099</t>
-  </si>
-  <si>
-    <t>LP-044472</t>
-  </si>
-  <si>
-    <t>LP-044474</t>
-  </si>
-  <si>
-    <t>LP-046657</t>
-  </si>
-  <si>
-    <t>LP-047013</t>
-  </si>
-  <si>
-    <t>LP-047015</t>
-  </si>
-  <si>
-    <t>LP-047137</t>
-  </si>
-  <si>
-    <t>LP-047139</t>
-  </si>
-  <si>
-    <t>LP-047140</t>
-  </si>
-  <si>
-    <t>LP-047141</t>
-  </si>
-  <si>
-    <t>LP-047142</t>
-  </si>
-  <si>
-    <t>LP-047143</t>
-  </si>
-  <si>
-    <t>LP-047225</t>
-  </si>
-  <si>
-    <t>LP-047282</t>
-  </si>
-  <si>
-    <t>LP-047315</t>
-  </si>
-  <si>
-    <t>LP-047418</t>
-  </si>
-  <si>
-    <t>LP-047624</t>
-  </si>
-  <si>
-    <t>LP-047651</t>
-  </si>
-  <si>
-    <t>LP-047713</t>
-  </si>
-  <si>
-    <t>LP-047912</t>
-  </si>
-  <si>
-    <t>LP-043008</t>
-  </si>
-  <si>
-    <t>LP-048112</t>
-  </si>
-  <si>
-    <t>LP-048113</t>
-  </si>
-  <si>
-    <t>LP-048242</t>
-  </si>
-  <si>
-    <t>LP-048243</t>
-  </si>
-  <si>
-    <t>LP-048247</t>
-  </si>
-  <si>
-    <t>LP-048300</t>
-  </si>
-  <si>
-    <t>LP-048443</t>
-  </si>
-  <si>
-    <t>LP-048499</t>
-  </si>
-  <si>
-    <t>LP-048514</t>
-  </si>
-  <si>
-    <t>LP-048527</t>
-  </si>
-  <si>
-    <t>LP-048528</t>
-  </si>
-  <si>
-    <t>LP-048530</t>
-  </si>
-  <si>
-    <t>LP-048531</t>
-  </si>
-  <si>
-    <t>LP-048632</t>
-  </si>
-  <si>
-    <t>LP-048637</t>
-  </si>
-  <si>
-    <t>LP-048671</t>
-  </si>
-  <si>
-    <t>LP-048843</t>
-  </si>
-  <si>
-    <t>LP-048844</t>
-  </si>
-  <si>
-    <t>LP-048845</t>
-  </si>
-  <si>
-    <t>LP-048849</t>
-  </si>
-  <si>
-    <t>LP-049060</t>
-  </si>
-  <si>
-    <t>LP-049061</t>
-  </si>
-  <si>
-    <t>LP-046637</t>
-  </si>
-  <si>
-    <t>LP-047138</t>
-  </si>
-  <si>
-    <t>LP-047531</t>
-  </si>
-  <si>
-    <t>LP-047534</t>
-  </si>
-  <si>
-    <t>LP-047902</t>
-  </si>
-  <si>
-    <t>LP-047956</t>
-  </si>
-  <si>
-    <t>LP-047993</t>
-  </si>
-  <si>
-    <t>LP-048115</t>
-  </si>
-  <si>
-    <t>LP-048116</t>
-  </si>
-  <si>
-    <t>LP-048130</t>
-  </si>
-  <si>
-    <t>LP-048236</t>
-  </si>
-  <si>
-    <t>LP-048241</t>
-  </si>
-  <si>
-    <t>LP-048335</t>
-  </si>
-  <si>
-    <t>LP-048336</t>
-  </si>
-  <si>
-    <t>LP-048341</t>
-  </si>
-  <si>
-    <t>LP-048342</t>
-  </si>
-  <si>
-    <t>LP-048442</t>
-  </si>
-  <si>
-    <t>LP-048529</t>
-  </si>
-  <si>
-    <t>LP-048535</t>
-  </si>
-  <si>
-    <t>LP-048538</t>
-  </si>
-  <si>
-    <t>LP-048539</t>
-  </si>
-  <si>
-    <t>LP-048541</t>
-  </si>
-  <si>
-    <t>LP-048573</t>
-  </si>
-  <si>
-    <t>LP-048947</t>
-  </si>
-  <si>
-    <t>LP-048948</t>
-  </si>
-  <si>
-    <t>LP-048958</t>
-  </si>
-  <si>
-    <t>LP-049276</t>
-  </si>
-  <si>
-    <t>LP-043682</t>
-  </si>
-  <si>
-    <t>LP-048246</t>
-  </si>
-  <si>
-    <t>LP-048521</t>
-  </si>
-  <si>
-    <t>LP-048536</t>
-  </si>
-  <si>
-    <t>LP-048668</t>
-  </si>
-  <si>
-    <t>LP-047904</t>
-  </si>
-  <si>
-    <t>LP-048534</t>
-  </si>
-  <si>
-    <t>LP-048624</t>
-  </si>
-  <si>
-    <t>LP-047532</t>
-  </si>
-  <si>
-    <t>LP-047711</t>
-  </si>
-  <si>
-    <t>LP-048114</t>
-  </si>
-  <si>
-    <t>LP-048129</t>
+    <t>LP-041219</t>
+  </si>
+  <si>
+    <t>LP-044566</t>
+  </si>
+  <si>
+    <t>LP-044569</t>
+  </si>
+  <si>
+    <t>LP-045431</t>
+  </si>
+  <si>
+    <t>LP-045457</t>
+  </si>
+  <si>
+    <t>LP-046299</t>
+  </si>
+  <si>
+    <t>LP-046300</t>
+  </si>
+  <si>
+    <t>LP-046302</t>
+  </si>
+  <si>
+    <t>LP-046304</t>
+  </si>
+  <si>
+    <t>LP-046306</t>
+  </si>
+  <si>
+    <t>LP-046392</t>
+  </si>
+  <si>
+    <t>LP-046491</t>
+  </si>
+  <si>
+    <t>LP-046535</t>
+  </si>
+  <si>
+    <t>LP-046723</t>
+  </si>
+  <si>
+    <t>LP-047082</t>
+  </si>
+  <si>
+    <t>LP-047157</t>
+  </si>
+  <si>
+    <t>LP-047222</t>
+  </si>
+  <si>
+    <t>LP-047278</t>
+  </si>
+  <si>
+    <t>LP-047403</t>
+  </si>
+  <si>
+    <t>LP-047417</t>
+  </si>
+  <si>
+    <t>LP-047561</t>
+  </si>
+  <si>
+    <t>LP-047642</t>
+  </si>
+  <si>
+    <t>LP-047894</t>
+  </si>
+  <si>
+    <t>LP-047919</t>
+  </si>
+  <si>
+    <t>LP-047924</t>
+  </si>
+  <si>
+    <t>LP-047949</t>
+  </si>
+  <si>
+    <t>LP-047953</t>
+  </si>
+  <si>
+    <t>LP-047972</t>
+  </si>
+  <si>
+    <t>LP-048062</t>
+  </si>
+  <si>
+    <t>LP-048082</t>
+  </si>
+  <si>
+    <t>LP-048085</t>
+  </si>
+  <si>
+    <t>LP-048283</t>
+  </si>
+  <si>
+    <t>LP-048290</t>
+  </si>
+  <si>
+    <t>LP-048331</t>
+  </si>
+  <si>
+    <t>LP-048450</t>
+  </si>
+  <si>
+    <t>LP-048490</t>
+  </si>
+  <si>
+    <t>LP-048513</t>
+  </si>
+  <si>
+    <t>LP-048725</t>
+  </si>
+  <si>
+    <t>LP-048726</t>
+  </si>
+  <si>
+    <t>LP-048728</t>
+  </si>
+  <si>
+    <t>LP-048730</t>
+  </si>
+  <si>
+    <t>LP-048748</t>
+  </si>
+  <si>
+    <t>LP-048764</t>
+  </si>
+  <si>
+    <t>LP-048825</t>
+  </si>
+  <si>
+    <t>LP-048835</t>
+  </si>
+  <si>
+    <t>LP-048869</t>
+  </si>
+  <si>
+    <t>LP-048875</t>
+  </si>
+  <si>
+    <t>LP-048877</t>
+  </si>
+  <si>
+    <t>LP-048899</t>
+  </si>
+  <si>
+    <t>LP-048919</t>
+  </si>
+  <si>
+    <t>LP-048955</t>
+  </si>
+  <si>
+    <t>LP-048991</t>
+  </si>
+  <si>
+    <t>LP-048992</t>
+  </si>
+  <si>
+    <t>LP-049076</t>
+  </si>
+  <si>
+    <t>LP-049101</t>
+  </si>
+  <si>
+    <t>LP-049136</t>
+  </si>
+  <si>
+    <t>LP-049137</t>
+  </si>
+  <si>
+    <t>LP-049198</t>
+  </si>
+  <si>
+    <t>LP-049215</t>
+  </si>
+  <si>
+    <t>LP-049228</t>
+  </si>
+  <si>
+    <t>LP-049229</t>
+  </si>
+  <si>
+    <t>LP-049272</t>
+  </si>
+  <si>
+    <t>LP-049289</t>
+  </si>
+  <si>
+    <t>LP-049397</t>
+  </si>
+  <si>
+    <t>LP-047960</t>
+  </si>
+  <si>
+    <t>LP-048464</t>
+  </si>
+  <si>
+    <t>LP-048545</t>
+  </si>
+  <si>
+    <t>LP-048731</t>
+  </si>
+  <si>
+    <t>LP-048928</t>
+  </si>
+  <si>
+    <t>LP-048952</t>
   </si>
 </sst>
 </file>
@@ -643,7 +598,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B86"/>
+  <dimension ref="A1:B71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -672,417 +627,342 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: updated and used PDF readers code
</commit_message>
<xml_diff>
--- a/Open-LPs - deitado.xlsx
+++ b/Open-LPs - deitado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6664EC-AAFB-4163-A7CA-AA7F28E85E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468D2A4F-2A11-4526-B98D-D9E1D64F742C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
   <si>
     <t>LP</t>
   </si>
@@ -28,214 +28,301 @@
     <t>Status</t>
   </si>
   <si>
-    <t>LP-041219</t>
-  </si>
-  <si>
-    <t>LP-044566</t>
-  </si>
-  <si>
-    <t>LP-044569</t>
-  </si>
-  <si>
-    <t>LP-045431</t>
-  </si>
-  <si>
-    <t>LP-045457</t>
-  </si>
-  <si>
-    <t>LP-046299</t>
-  </si>
-  <si>
-    <t>LP-046300</t>
-  </si>
-  <si>
-    <t>LP-046302</t>
-  </si>
-  <si>
-    <t>LP-046304</t>
-  </si>
-  <si>
-    <t>LP-046306</t>
-  </si>
-  <si>
-    <t>LP-046392</t>
-  </si>
-  <si>
-    <t>LP-046491</t>
-  </si>
-  <si>
-    <t>LP-046535</t>
-  </si>
-  <si>
-    <t>LP-046723</t>
-  </si>
-  <si>
-    <t>LP-047082</t>
-  </si>
-  <si>
-    <t>LP-047157</t>
-  </si>
-  <si>
-    <t>LP-047222</t>
-  </si>
-  <si>
-    <t>LP-047278</t>
-  </si>
-  <si>
-    <t>LP-047403</t>
-  </si>
-  <si>
-    <t>LP-047417</t>
-  </si>
-  <si>
-    <t>LP-047561</t>
-  </si>
-  <si>
-    <t>LP-047642</t>
-  </si>
-  <si>
-    <t>LP-047894</t>
-  </si>
-  <si>
-    <t>LP-047919</t>
-  </si>
-  <si>
-    <t>LP-047924</t>
-  </si>
-  <si>
-    <t>LP-047949</t>
-  </si>
-  <si>
-    <t>LP-047953</t>
-  </si>
-  <si>
-    <t>LP-047972</t>
-  </si>
-  <si>
-    <t>LP-048062</t>
-  </si>
-  <si>
-    <t>LP-048082</t>
-  </si>
-  <si>
-    <t>LP-048085</t>
-  </si>
-  <si>
-    <t>LP-048283</t>
-  </si>
-  <si>
-    <t>LP-048290</t>
-  </si>
-  <si>
-    <t>LP-048331</t>
-  </si>
-  <si>
-    <t>LP-048450</t>
-  </si>
-  <si>
-    <t>LP-048490</t>
-  </si>
-  <si>
-    <t>LP-048513</t>
-  </si>
-  <si>
-    <t>LP-048725</t>
-  </si>
-  <si>
-    <t>LP-048726</t>
-  </si>
-  <si>
-    <t>LP-048728</t>
-  </si>
-  <si>
-    <t>LP-048730</t>
-  </si>
-  <si>
-    <t>LP-048748</t>
-  </si>
-  <si>
-    <t>LP-048764</t>
-  </si>
-  <si>
-    <t>LP-048825</t>
-  </si>
-  <si>
-    <t>LP-048835</t>
-  </si>
-  <si>
-    <t>LP-048869</t>
-  </si>
-  <si>
-    <t>LP-048875</t>
-  </si>
-  <si>
-    <t>LP-048877</t>
-  </si>
-  <si>
-    <t>LP-048899</t>
-  </si>
-  <si>
-    <t>LP-048919</t>
-  </si>
-  <si>
-    <t>LP-048955</t>
-  </si>
-  <si>
-    <t>LP-048991</t>
-  </si>
-  <si>
-    <t>LP-048992</t>
-  </si>
-  <si>
-    <t>LP-049076</t>
-  </si>
-  <si>
-    <t>LP-049101</t>
-  </si>
-  <si>
-    <t>LP-049136</t>
-  </si>
-  <si>
-    <t>LP-049137</t>
-  </si>
-  <si>
-    <t>LP-049198</t>
-  </si>
-  <si>
-    <t>LP-049215</t>
-  </si>
-  <si>
-    <t>LP-049228</t>
-  </si>
-  <si>
-    <t>LP-049229</t>
-  </si>
-  <si>
-    <t>LP-049272</t>
-  </si>
-  <si>
-    <t>LP-049289</t>
-  </si>
-  <si>
-    <t>LP-049397</t>
-  </si>
-  <si>
-    <t>LP-047960</t>
-  </si>
-  <si>
-    <t>LP-048464</t>
-  </si>
-  <si>
-    <t>LP-048545</t>
-  </si>
-  <si>
-    <t>LP-048731</t>
-  </si>
-  <si>
-    <t>LP-048928</t>
-  </si>
-  <si>
-    <t>LP-048952</t>
+    <t>LP-041570</t>
+  </si>
+  <si>
+    <t>LP-042368</t>
+  </si>
+  <si>
+    <t>LP-043866</t>
+  </si>
+  <si>
+    <t>LP-043880</t>
+  </si>
+  <si>
+    <t>LP-043886</t>
+  </si>
+  <si>
+    <t>LP-044154</t>
+  </si>
+  <si>
+    <t>LP-044463</t>
+  </si>
+  <si>
+    <t>LP-044469</t>
+  </si>
+  <si>
+    <t>LP-045184</t>
+  </si>
+  <si>
+    <t>LP-045223</t>
+  </si>
+  <si>
+    <t>LP-045899</t>
+  </si>
+  <si>
+    <t>LP-046168</t>
+  </si>
+  <si>
+    <t>LP-046301</t>
+  </si>
+  <si>
+    <t>LP-046303</t>
+  </si>
+  <si>
+    <t>LP-046305</t>
+  </si>
+  <si>
+    <t>LP-046445</t>
+  </si>
+  <si>
+    <t>LP-046446</t>
+  </si>
+  <si>
+    <t>LP-046447</t>
+  </si>
+  <si>
+    <t>LP-046448</t>
+  </si>
+  <si>
+    <t>LP-046497</t>
+  </si>
+  <si>
+    <t>LP-046518</t>
+  </si>
+  <si>
+    <t>LP-046899</t>
+  </si>
+  <si>
+    <t>LP-046968</t>
+  </si>
+  <si>
+    <t>LP-047159</t>
+  </si>
+  <si>
+    <t>LP-047215</t>
+  </si>
+  <si>
+    <t>LP-047328</t>
+  </si>
+  <si>
+    <t>LP-047637</t>
+  </si>
+  <si>
+    <t>LP-047666</t>
+  </si>
+  <si>
+    <t>LP-047667</t>
+  </si>
+  <si>
+    <t>LP-047804</t>
+  </si>
+  <si>
+    <t>LP-047864</t>
+  </si>
+  <si>
+    <t>LP-047940</t>
+  </si>
+  <si>
+    <t>LP-047963</t>
+  </si>
+  <si>
+    <t>LP-047965</t>
+  </si>
+  <si>
+    <t>LP-048021</t>
+  </si>
+  <si>
+    <t>LP-048024</t>
+  </si>
+  <si>
+    <t>LP-048079</t>
+  </si>
+  <si>
+    <t>LP-048080</t>
+  </si>
+  <si>
+    <t>LP-048118</t>
+  </si>
+  <si>
+    <t>LP-048217</t>
+  </si>
+  <si>
+    <t>LP-048258</t>
+  </si>
+  <si>
+    <t>LP-048281</t>
+  </si>
+  <si>
+    <t>LP-048282</t>
+  </si>
+  <si>
+    <t>LP-048334</t>
+  </si>
+  <si>
+    <t>LP-048360</t>
+  </si>
+  <si>
+    <t>LP-048439</t>
+  </si>
+  <si>
+    <t>LP-048440</t>
+  </si>
+  <si>
+    <t>LP-048445</t>
+  </si>
+  <si>
+    <t>LP-048457</t>
+  </si>
+  <si>
+    <t>LP-048458</t>
+  </si>
+  <si>
+    <t>LP-048485</t>
+  </si>
+  <si>
+    <t>LP-048526</t>
+  </si>
+  <si>
+    <t>LP-048543</t>
+  </si>
+  <si>
+    <t>LP-048719</t>
+  </si>
+  <si>
+    <t>LP-048721</t>
+  </si>
+  <si>
+    <t>LP-048722</t>
+  </si>
+  <si>
+    <t>LP-048747</t>
+  </si>
+  <si>
+    <t>LP-048763</t>
+  </si>
+  <si>
+    <t>LP-048765</t>
+  </si>
+  <si>
+    <t>LP-048766</t>
+  </si>
+  <si>
+    <t>LP-048828</t>
+  </si>
+  <si>
+    <t>LP-048832</t>
+  </si>
+  <si>
+    <t>LP-048833</t>
+  </si>
+  <si>
+    <t>LP-048862</t>
+  </si>
+  <si>
+    <t>LP-048892</t>
+  </si>
+  <si>
+    <t>LP-048903</t>
+  </si>
+  <si>
+    <t>LP-048904</t>
+  </si>
+  <si>
+    <t>LP-048911</t>
+  </si>
+  <si>
+    <t>LP-048917</t>
+  </si>
+  <si>
+    <t>LP-048931</t>
+  </si>
+  <si>
+    <t>LP-048936</t>
+  </si>
+  <si>
+    <t>LP-048940</t>
+  </si>
+  <si>
+    <t>LP-048942</t>
+  </si>
+  <si>
+    <t>LP-048954</t>
+  </si>
+  <si>
+    <t>LP-049024</t>
+  </si>
+  <si>
+    <t>LP-049051</t>
+  </si>
+  <si>
+    <t>LP-049059</t>
+  </si>
+  <si>
+    <t>LP-049146</t>
+  </si>
+  <si>
+    <t>LP-049147</t>
+  </si>
+  <si>
+    <t>LP-049185</t>
+  </si>
+  <si>
+    <t>LP-049205</t>
+  </si>
+  <si>
+    <t>LP-049248</t>
+  </si>
+  <si>
+    <t>LP-049250</t>
+  </si>
+  <si>
+    <t>LP-049253</t>
+  </si>
+  <si>
+    <t>LP-049274</t>
+  </si>
+  <si>
+    <t>LP-049445</t>
+  </si>
+  <si>
+    <t>LP-049548</t>
+  </si>
+  <si>
+    <t>LP-049557</t>
+  </si>
+  <si>
+    <t>LP-049586</t>
+  </si>
+  <si>
+    <t>LP-049587</t>
+  </si>
+  <si>
+    <t>LP-049595</t>
+  </si>
+  <si>
+    <t>LP-049623</t>
+  </si>
+  <si>
+    <t>LP-048372</t>
+  </si>
+  <si>
+    <t>LP-049075</t>
+  </si>
+  <si>
+    <t>LP-049239</t>
+  </si>
+  <si>
+    <t>LP-049263</t>
+  </si>
+  <si>
+    <t>LP-049267</t>
+  </si>
+  <si>
+    <t>LP-049492</t>
+  </si>
+  <si>
+    <t>LP-049705</t>
   </si>
 </sst>
 </file>
@@ -598,14 +685,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -752,37 +838,37 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -797,172 +883,322 @@
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>65</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
used: LP&OM - KW22/23 finished
</commit_message>
<xml_diff>
--- a/Open-LPs - deitado.xlsx
+++ b/Open-LPs - deitado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B5B254-F495-483B-B156-AC82F4DCB508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BD8047-E4D8-4B0C-94C7-5E389ECA82FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>LP</t>
   </si>
@@ -28,100 +28,196 @@
     <t>Status</t>
   </si>
   <si>
-    <t>LP-043681</t>
-  </si>
-  <si>
-    <t>LP-043683</t>
-  </si>
-  <si>
-    <t>LP-045106</t>
-  </si>
-  <si>
-    <t>LP-045221</t>
-  </si>
-  <si>
-    <t>LP-047165</t>
-  </si>
-  <si>
-    <t>LP-047213</t>
-  </si>
-  <si>
-    <t>LP-047668</t>
-  </si>
-  <si>
-    <t>LP-047669</t>
-  </si>
-  <si>
-    <t>LP-047670</t>
-  </si>
-  <si>
-    <t>LP-047738</t>
-  </si>
-  <si>
-    <t>LP-047851</t>
-  </si>
-  <si>
-    <t>LP-048072</t>
-  </si>
-  <si>
-    <t>LP-048128</t>
-  </si>
-  <si>
-    <t>LP-048131</t>
-  </si>
-  <si>
-    <t>LP-048215</t>
-  </si>
-  <si>
-    <t>LP-048245</t>
-  </si>
-  <si>
-    <t>LP-048284</t>
-  </si>
-  <si>
-    <t>LP-048417</t>
-  </si>
-  <si>
-    <t>LP-048500</t>
-  </si>
-  <si>
-    <t>LP-048837</t>
-  </si>
-  <si>
-    <t>LP-048911</t>
-  </si>
-  <si>
-    <t>LP-049111</t>
-  </si>
-  <si>
-    <t>LP-049270</t>
-  </si>
-  <si>
-    <t>LP-049308</t>
-  </si>
-  <si>
-    <t>LP-049560</t>
-  </si>
-  <si>
-    <t>LP-049566</t>
-  </si>
-  <si>
-    <t>LP-049589</t>
-  </si>
-  <si>
-    <t>LP-049593</t>
-  </si>
-  <si>
-    <t>LP-049632</t>
-  </si>
-  <si>
-    <t>LP-049633</t>
-  </si>
-  <si>
-    <t>LP-049753</t>
-  </si>
-  <si>
-    <t>LP-049591</t>
+    <t>LP-046106</t>
+  </si>
+  <si>
+    <t>LP-046491</t>
+  </si>
+  <si>
+    <t>LP-046503</t>
+  </si>
+  <si>
+    <t>LP-046530</t>
+  </si>
+  <si>
+    <t>LP-046841</t>
+  </si>
+  <si>
+    <t>LP-047126</t>
+  </si>
+  <si>
+    <t>LP-047162</t>
+  </si>
+  <si>
+    <t>LP-047230</t>
+  </si>
+  <si>
+    <t>LP-047254</t>
+  </si>
+  <si>
+    <t>LP-047323</t>
+  </si>
+  <si>
+    <t>LP-047363</t>
+  </si>
+  <si>
+    <t>LP-047663</t>
+  </si>
+  <si>
+    <t>LP-047925</t>
+  </si>
+  <si>
+    <t>LP-048000</t>
+  </si>
+  <si>
+    <t>LP-048053</t>
+  </si>
+  <si>
+    <t>LP-048317</t>
+  </si>
+  <si>
+    <t>LP-048329</t>
+  </si>
+  <si>
+    <t>LP-048544</t>
+  </si>
+  <si>
+    <t>LP-048679</t>
+  </si>
+  <si>
+    <t>LP-048681</t>
+  </si>
+  <si>
+    <t>LP-048683</t>
+  </si>
+  <si>
+    <t>LP-048685</t>
+  </si>
+  <si>
+    <t>LP-048812</t>
+  </si>
+  <si>
+    <t>LP-048829</t>
+  </si>
+  <si>
+    <t>LP-048834</t>
+  </si>
+  <si>
+    <t>LP-048836</t>
+  </si>
+  <si>
+    <t>LP-048870</t>
+  </si>
+  <si>
+    <t>LP-048880</t>
+  </si>
+  <si>
+    <t>LP-048881</t>
+  </si>
+  <si>
+    <t>LP-048890</t>
+  </si>
+  <si>
+    <t>LP-048891</t>
+  </si>
+  <si>
+    <t>LP-048915</t>
+  </si>
+  <si>
+    <t>LP-048924</t>
+  </si>
+  <si>
+    <t>LP-048933</t>
+  </si>
+  <si>
+    <t>LP-048934</t>
+  </si>
+  <si>
+    <t>LP-048935</t>
+  </si>
+  <si>
+    <t>LP-048938</t>
+  </si>
+  <si>
+    <t>LP-049025</t>
+  </si>
+  <si>
+    <t>LP-049127</t>
+  </si>
+  <si>
+    <t>LP-049181</t>
+  </si>
+  <si>
+    <t>LP-049182</t>
+  </si>
+  <si>
+    <t>LP-049183</t>
+  </si>
+  <si>
+    <t>LP-049184</t>
+  </si>
+  <si>
+    <t>LP-049219</t>
+  </si>
+  <si>
+    <t>LP-049237</t>
+  </si>
+  <si>
+    <t>LP-049238</t>
+  </si>
+  <si>
+    <t>LP-049282</t>
+  </si>
+  <si>
+    <t>LP-049419</t>
+  </si>
+  <si>
+    <t>LP-049420</t>
+  </si>
+  <si>
+    <t>LP-049422</t>
+  </si>
+  <si>
+    <t>LP-049424</t>
+  </si>
+  <si>
+    <t>LP-049426</t>
+  </si>
+  <si>
+    <t>LP-049440</t>
+  </si>
+  <si>
+    <t>LP-049471</t>
+  </si>
+  <si>
+    <t>LP-049546</t>
+  </si>
+  <si>
+    <t>LP-049634</t>
+  </si>
+  <si>
+    <t>LP-049635</t>
+  </si>
+  <si>
+    <t>LP-049795</t>
+  </si>
+  <si>
+    <t>LP-049796</t>
+  </si>
+  <si>
+    <t>LP-049991</t>
+  </si>
+  <si>
+    <t>LP-047671</t>
+  </si>
+  <si>
+    <t>LP-048675</t>
+  </si>
+  <si>
+    <t>LP-048677</t>
+  </si>
+  <si>
+    <t>LP-050021</t>
   </si>
 </sst>
 </file>
@@ -484,7 +580,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -564,102 +660,262 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
used: Finish LP and OM used
</commit_message>
<xml_diff>
--- a/Open-LPs - deitado.xlsx
+++ b/Open-LPs - deitado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BD8047-E4D8-4B0C-94C7-5E389ECA82FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49ECF1E0-3765-4434-A80A-5972D259971E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>LP</t>
   </si>
@@ -28,196 +28,172 @@
     <t>Status</t>
   </si>
   <si>
-    <t>LP-046106</t>
-  </si>
-  <si>
-    <t>LP-046491</t>
-  </si>
-  <si>
-    <t>LP-046503</t>
-  </si>
-  <si>
-    <t>LP-046530</t>
-  </si>
-  <si>
-    <t>LP-046841</t>
-  </si>
-  <si>
-    <t>LP-047126</t>
-  </si>
-  <si>
-    <t>LP-047162</t>
-  </si>
-  <si>
-    <t>LP-047230</t>
-  </si>
-  <si>
-    <t>LP-047254</t>
-  </si>
-  <si>
-    <t>LP-047323</t>
-  </si>
-  <si>
-    <t>LP-047363</t>
-  </si>
-  <si>
-    <t>LP-047663</t>
-  </si>
-  <si>
-    <t>LP-047925</t>
-  </si>
-  <si>
-    <t>LP-048000</t>
-  </si>
-  <si>
-    <t>LP-048053</t>
-  </si>
-  <si>
-    <t>LP-048317</t>
-  </si>
-  <si>
-    <t>LP-048329</t>
-  </si>
-  <si>
-    <t>LP-048544</t>
-  </si>
-  <si>
-    <t>LP-048679</t>
-  </si>
-  <si>
-    <t>LP-048681</t>
-  </si>
-  <si>
-    <t>LP-048683</t>
-  </si>
-  <si>
-    <t>LP-048685</t>
-  </si>
-  <si>
-    <t>LP-048812</t>
-  </si>
-  <si>
-    <t>LP-048829</t>
-  </si>
-  <si>
-    <t>LP-048834</t>
-  </si>
-  <si>
-    <t>LP-048836</t>
-  </si>
-  <si>
-    <t>LP-048870</t>
-  </si>
-  <si>
-    <t>LP-048880</t>
-  </si>
-  <si>
-    <t>LP-048881</t>
-  </si>
-  <si>
-    <t>LP-048890</t>
-  </si>
-  <si>
-    <t>LP-048891</t>
-  </si>
-  <si>
-    <t>LP-048915</t>
-  </si>
-  <si>
-    <t>LP-048924</t>
-  </si>
-  <si>
-    <t>LP-048933</t>
-  </si>
-  <si>
-    <t>LP-048934</t>
-  </si>
-  <si>
-    <t>LP-048935</t>
-  </si>
-  <si>
-    <t>LP-048938</t>
-  </si>
-  <si>
-    <t>LP-049025</t>
-  </si>
-  <si>
-    <t>LP-049127</t>
-  </si>
-  <si>
-    <t>LP-049181</t>
-  </si>
-  <si>
-    <t>LP-049182</t>
-  </si>
-  <si>
-    <t>LP-049183</t>
-  </si>
-  <si>
-    <t>LP-049184</t>
-  </si>
-  <si>
-    <t>LP-049219</t>
-  </si>
-  <si>
-    <t>LP-049237</t>
-  </si>
-  <si>
-    <t>LP-049238</t>
-  </si>
-  <si>
-    <t>LP-049282</t>
-  </si>
-  <si>
-    <t>LP-049419</t>
-  </si>
-  <si>
-    <t>LP-049420</t>
-  </si>
-  <si>
-    <t>LP-049422</t>
-  </si>
-  <si>
-    <t>LP-049424</t>
-  </si>
-  <si>
-    <t>LP-049426</t>
-  </si>
-  <si>
-    <t>LP-049440</t>
-  </si>
-  <si>
-    <t>LP-049471</t>
-  </si>
-  <si>
-    <t>LP-049546</t>
-  </si>
-  <si>
-    <t>LP-049634</t>
-  </si>
-  <si>
-    <t>LP-049635</t>
-  </si>
-  <si>
-    <t>LP-049795</t>
-  </si>
-  <si>
-    <t>LP-049796</t>
-  </si>
-  <si>
-    <t>LP-049991</t>
-  </si>
-  <si>
-    <t>LP-047671</t>
-  </si>
-  <si>
-    <t>LP-048675</t>
-  </si>
-  <si>
-    <t>LP-048677</t>
-  </si>
-  <si>
-    <t>LP-050021</t>
+    <t>LP-046493</t>
+  </si>
+  <si>
+    <t>LP-046901</t>
+  </si>
+  <si>
+    <t>LP-047152</t>
+  </si>
+  <si>
+    <t>LP-047229</t>
+  </si>
+  <si>
+    <t>LP-047292</t>
+  </si>
+  <si>
+    <t>LP-048007</t>
+  </si>
+  <si>
+    <t>LP-048077</t>
+  </si>
+  <si>
+    <t>LP-048117</t>
+  </si>
+  <si>
+    <t>LP-048216</t>
+  </si>
+  <si>
+    <t>LP-048285</t>
+  </si>
+  <si>
+    <t>LP-048330</t>
+  </si>
+  <si>
+    <t>LP-048337</t>
+  </si>
+  <si>
+    <t>LP-048548</t>
+  </si>
+  <si>
+    <t>LP-048656</t>
+  </si>
+  <si>
+    <t>LP-048673</t>
+  </si>
+  <si>
+    <t>LP-048830</t>
+  </si>
+  <si>
+    <t>LP-048831</t>
+  </si>
+  <si>
+    <t>LP-048871</t>
+  </si>
+  <si>
+    <t>LP-048872</t>
+  </si>
+  <si>
+    <t>LP-048898</t>
+  </si>
+  <si>
+    <t>LP-048908</t>
+  </si>
+  <si>
+    <t>LP-048929</t>
+  </si>
+  <si>
+    <t>LP-048965</t>
+  </si>
+  <si>
+    <t>LP-049058</t>
+  </si>
+  <si>
+    <t>LP-049102</t>
+  </si>
+  <si>
+    <t>LP-049169</t>
+  </si>
+  <si>
+    <t>LP-049236</t>
+  </si>
+  <si>
+    <t>LP-049243</t>
+  </si>
+  <si>
+    <t>LP-049245</t>
+  </si>
+  <si>
+    <t>LP-049261</t>
+  </si>
+  <si>
+    <t>LP-049280</t>
+  </si>
+  <si>
+    <t>LP-049415</t>
+  </si>
+  <si>
+    <t>LP-049423</t>
+  </si>
+  <si>
+    <t>LP-049434</t>
+  </si>
+  <si>
+    <t>LP-049437</t>
+  </si>
+  <si>
+    <t>LP-049555</t>
+  </si>
+  <si>
+    <t>LP-049595</t>
+  </si>
+  <si>
+    <t>LP-049630</t>
+  </si>
+  <si>
+    <t>LP-049638</t>
+  </si>
+  <si>
+    <t>LP-049654</t>
+  </si>
+  <si>
+    <t>LP-049706</t>
+  </si>
+  <si>
+    <t>LP-049712</t>
+  </si>
+  <si>
+    <t>LP-049745</t>
+  </si>
+  <si>
+    <t>LP-049793</t>
+  </si>
+  <si>
+    <t>LP-049875</t>
+  </si>
+  <si>
+    <t>LP-049898</t>
+  </si>
+  <si>
+    <t>LP-049904</t>
+  </si>
+  <si>
+    <t>LP-049917</t>
+  </si>
+  <si>
+    <t>LP-049998</t>
+  </si>
+  <si>
+    <t>LP-050117</t>
+  </si>
+  <si>
+    <t>LP-050162</t>
+  </si>
+  <si>
+    <t>LP-043640</t>
+  </si>
+  <si>
+    <t>LP-047426</t>
+  </si>
+  <si>
+    <t>LP-048937</t>
+  </si>
+  <si>
+    <t>LP-049021</t>
+  </si>
+  <si>
+    <t>LP-049567</t>
   </si>
 </sst>
 </file>
@@ -580,7 +556,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -600,127 +576,127 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
@@ -730,192 +706,152 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
used: Finish LPs and OMs
</commit_message>
<xml_diff>
--- a/Open-LPs - deitado.xlsx
+++ b/Open-LPs - deitado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946040B5-8272-4CA7-AFF9-E5845DDE2A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4376B4C-BF70-487F-A8CA-ADB2885D6B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,78 +20,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>LP</t>
   </si>
   <si>
-    <t>LP-040924</t>
-  </si>
-  <si>
-    <t>LP-045267</t>
-  </si>
-  <si>
-    <t>LP-045871</t>
-  </si>
-  <si>
-    <t>LP-046516</t>
-  </si>
-  <si>
-    <t>LP-047153</t>
-  </si>
-  <si>
-    <t>LP-047154</t>
-  </si>
-  <si>
-    <t>LP-047227</t>
-  </si>
-  <si>
-    <t>LP-047256</t>
-  </si>
-  <si>
-    <t>LP-047274</t>
-  </si>
-  <si>
-    <t>LP-047275</t>
-  </si>
-  <si>
-    <t>LP-047281</t>
-  </si>
-  <si>
-    <t>LP-047340</t>
-  </si>
-  <si>
-    <t>LP-047456</t>
-  </si>
-  <si>
-    <t>LP-048176</t>
-  </si>
-  <si>
-    <t>LP-048856</t>
-  </si>
-  <si>
-    <t>LP-048894</t>
-  </si>
-  <si>
-    <t>LP-048930</t>
-  </si>
-  <si>
-    <t>LP-049338</t>
-  </si>
-  <si>
-    <t>LP-049381</t>
-  </si>
-  <si>
-    <t>LP-049470</t>
-  </si>
-  <si>
-    <t>LP-045900</t>
-  </si>
-  <si>
-    <t>LP-048839</t>
-  </si>
-  <si>
-    <t>LP-049235</t>
+    <t>LP-032383</t>
+  </si>
+  <si>
+    <t>LP-044468</t>
+  </si>
+  <si>
+    <t>LP-047127</t>
+  </si>
+  <si>
+    <t>LP-047276</t>
+  </si>
+  <si>
+    <t>LP-047425</t>
+  </si>
+  <si>
+    <t>LP-047636</t>
+  </si>
+  <si>
+    <t>LP-048244</t>
+  </si>
+  <si>
+    <t>LP-048301</t>
+  </si>
+  <si>
+    <t>LP-048670</t>
+  </si>
+  <si>
+    <t>LP-048674</t>
+  </si>
+  <si>
+    <t>LP-048746</t>
+  </si>
+  <si>
+    <t>LP-048932</t>
+  </si>
+  <si>
+    <t>LP-049427</t>
+  </si>
+  <si>
+    <t>LP-049443</t>
+  </si>
+  <si>
+    <t>LP-049800</t>
+  </si>
+  <si>
+    <t>LP-050182</t>
+  </si>
+  <si>
+    <t>LP-050183</t>
+  </si>
+  <si>
+    <t>LP-050208</t>
+  </si>
+  <si>
+    <t>LP-043257</t>
+  </si>
+  <si>
+    <t>LP-049257</t>
   </si>
 </sst>
 </file>
@@ -454,11 +445,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -477,17 +466,17 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -537,17 +526,17 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -567,22 +556,7 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>